<commit_message>
added warnings and alerts and more logging to columns algorithm
</commit_message>
<xml_diff>
--- a/User Files/AnonymousUser_datafiles/Result DF Display.xlsx
+++ b/User Files/AnonymousUser_datafiles/Result DF Display.xlsx
@@ -37,7 +37,7 @@
     <t>mydate</t>
   </si>
   <si>
-    <t>fess</t>
+    <t>0010</t>
   </si>
   <si>
     <t>Celestia</t>
@@ -912,7 +912,7 @@
         <v>132</v>
       </c>
       <c r="H2">
-        <f>SUBSTITUTE(D2:D2,"@","")</f>
+        <f>IF(YEAR(G2:G2)&lt;2030, A2:A2, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -939,7 +939,7 @@
         <v>133</v>
       </c>
       <c r="H3">
-        <f>SUBSTITUTE(D3:D3,"@","")</f>
+        <f>IF(YEAR(G3:G3)&lt;2030, A3:A3, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -966,7 +966,7 @@
         <v>134</v>
       </c>
       <c r="H4">
-        <f>SUBSTITUTE(D4:D4,"@","")</f>
+        <f>IF(YEAR(G4:G4)&lt;2030, A4:A4, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -993,7 +993,7 @@
         <v>135</v>
       </c>
       <c r="H5">
-        <f>SUBSTITUTE(D5:D5,"@","")</f>
+        <f>IF(YEAR(G5:G5)&lt;2030, A5:A5, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
         <v>136</v>
       </c>
       <c r="H6">
-        <f>SUBSTITUTE(D6:D6,"@","")</f>
+        <f>IF(YEAR(G6:G6)&lt;2030, A6:A6, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
         <v>137</v>
       </c>
       <c r="H7">
-        <f>SUBSTITUTE(D7:D7,"@","")</f>
+        <f>IF(YEAR(G7:G7)&lt;2030, A7:A7, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
         <v>138</v>
       </c>
       <c r="H8">
-        <f>SUBSTITUTE(D8:D8,"@","")</f>
+        <f>IF(YEAR(G8:G8)&lt;2030, A8:A8, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
         <v>139</v>
       </c>
       <c r="H9">
-        <f>SUBSTITUTE(D9:D9,"@","")</f>
+        <f>IF(YEAR(G9:G9)&lt;2030, A9:A9, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
         <v>140</v>
       </c>
       <c r="H10">
-        <f>SUBSTITUTE(D10:D10,"@","")</f>
+        <f>IF(YEAR(G10:G10)&lt;2030, A10:A10, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
         <v>141</v>
       </c>
       <c r="H11">
-        <f>SUBSTITUTE(D11:D11,"@","")</f>
+        <f>IF(YEAR(G11:G11)&lt;2030, A11:A11, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
         <v>142</v>
       </c>
       <c r="H12">
-        <f>SUBSTITUTE(D12:D12,"@","")</f>
+        <f>IF(YEAR(G12:G12)&lt;2030, A12:A12, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
         <v>143</v>
       </c>
       <c r="H13">
-        <f>SUBSTITUTE(D13:D13,"@","")</f>
+        <f>IF(YEAR(G13:G13)&lt;2030, A13:A13, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
         <v>144</v>
       </c>
       <c r="H14">
-        <f>SUBSTITUTE(D14:D14,"@","")</f>
+        <f>IF(YEAR(G14:G14)&lt;2030, A14:A14, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
         <v>145</v>
       </c>
       <c r="H15">
-        <f>SUBSTITUTE(D15:D15,"@","")</f>
+        <f>IF(YEAR(G15:G15)&lt;2030, A15:A15, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
         <v>146</v>
       </c>
       <c r="H16">
-        <f>SUBSTITUTE(D16:D16,"@","")</f>
+        <f>IF(YEAR(G16:G16)&lt;2030, A16:A16, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
         <v>147</v>
       </c>
       <c r="H17">
-        <f>SUBSTITUTE(D17:D17,"@","")</f>
+        <f>IF(YEAR(G17:G17)&lt;2030, A17:A17, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
         <v>148</v>
       </c>
       <c r="H18">
-        <f>SUBSTITUTE(D18:D18,"@","")</f>
+        <f>IF(YEAR(G18:G18)&lt;2030, A18:A18, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
         <v>149</v>
       </c>
       <c r="H19">
-        <f>SUBSTITUTE(D19:D19,"@","")</f>
+        <f>IF(YEAR(G19:G19)&lt;2030, A19:A19, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
         <v>150</v>
       </c>
       <c r="H20">
-        <f>SUBSTITUTE(D20:D20,"@","")</f>
+        <f>IF(YEAR(G20:G20)&lt;2030, A20:A20, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
         <v>151</v>
       </c>
       <c r="H21">
-        <f>SUBSTITUTE(D21:D21,"@","")</f>
+        <f>IF(YEAR(G21:G21)&lt;2030, A21:A21, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1452,7 +1452,7 @@
         <v>152</v>
       </c>
       <c r="H22">
-        <f>SUBSTITUTE(D22:D22,"@","")</f>
+        <f>IF(YEAR(G22:G22)&lt;2030, A22:A22, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
         <v>153</v>
       </c>
       <c r="H23">
-        <f>SUBSTITUTE(D23:D23,"@","")</f>
+        <f>IF(YEAR(G23:G23)&lt;2030, A23:A23, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
         <v>154</v>
       </c>
       <c r="H24">
-        <f>SUBSTITUTE(D24:D24,"@","")</f>
+        <f>IF(YEAR(G24:G24)&lt;2030, A24:A24, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
         <v>155</v>
       </c>
       <c r="H25">
-        <f>SUBSTITUTE(D25:D25,"@","")</f>
+        <f>IF(YEAR(G25:G25)&lt;2030, A25:A25, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1560,7 +1560,7 @@
         <v>156</v>
       </c>
       <c r="H26">
-        <f>SUBSTITUTE(D26:D26,"@","")</f>
+        <f>IF(YEAR(G26:G26)&lt;2030, A26:A26, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
         <v>157</v>
       </c>
       <c r="H27">
-        <f>SUBSTITUTE(D27:D27,"@","")</f>
+        <f>IF(YEAR(G27:G27)&lt;2030, A27:A27, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
         <v>158</v>
       </c>
       <c r="H28">
-        <f>SUBSTITUTE(D28:D28,"@","")</f>
+        <f>IF(YEAR(G28:G28)&lt;2030, A28:A28, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
         <v>159</v>
       </c>
       <c r="H29">
-        <f>SUBSTITUTE(D29:D29,"@","")</f>
+        <f>IF(YEAR(G29:G29)&lt;2030, A29:A29, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1668,7 +1668,7 @@
         <v>160</v>
       </c>
       <c r="H30">
-        <f>SUBSTITUTE(D30:D30,"@","")</f>
+        <f>IF(YEAR(G30:G30)&lt;2030, A30:A30, "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
         <v>161</v>
       </c>
       <c r="H31">
-        <f>SUBSTITUTE(D31:D31,"@","")</f>
+        <f>IF(YEAR(G31:G31)&lt;2030, A31:A31, "")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>